<commit_message>
likelihood ratio testing and parameter uncertainty
</commit_message>
<xml_diff>
--- a/05.analyses/demography/dadi/1D/glob/models/dadi_glob1D_results_summary.xlsx
+++ b/05.analyses/demography/dadi/1D/glob/models/dadi_glob1D_results_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/05.analyses/demography/dadi/1D/glob/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89368558-88FD-491C-97B4-28AE2F3F0DBC}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="8_{21408352-E5DB-40D9-AE77-F269512CD883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3754CADB-A8AF-488F-A5B5-7C427937B8D9}"/>
   <bookViews>
-    <workbookView xWindow="-26760" yWindow="-7875" windowWidth="22695" windowHeight="12870" xr2:uid="{2A3D79EE-876F-4CC7-84D9-EA1A1596E616}"/>
+    <workbookView xWindow="1308" yWindow="-108" windowWidth="21840" windowHeight="13176" activeTab="2" xr2:uid="{2A3D79EE-876F-4CC7-84D9-EA1A1596E616}"/>
   </bookViews>
   <sheets>
     <sheet name="all model results" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
   <si>
     <t>02.growth</t>
   </si>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>Three Epoch</t>
+  </si>
+  <si>
+    <t>UNCERTAINTY ESTIMATES</t>
+  </si>
+  <si>
+    <t>95% CONFIDENCE INTERVALS</t>
+  </si>
+  <si>
+    <t>Lower Bound</t>
+  </si>
+  <si>
+    <t>Upper Bound</t>
   </si>
 </sst>
 </file>
@@ -326,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +363,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -719,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -789,6 +807,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
@@ -801,27 +840,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1162,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1123D7EB-ECD6-4C25-BAEF-EFE90AE1E5C4}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,30 +1497,30 @@
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="F3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="61"/>
-      <c r="J3" s="60" t="s">
+      <c r="G3" s="53"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="61"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="57"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
@@ -1546,7 +1586,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="59" t="s">
         <v>28</v>
       </c>
       <c r="B6" t="s">
@@ -1563,7 +1603,7 @@
       <c r="H6" s="23">
         <v>10</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="59" t="s">
         <v>28</v>
       </c>
       <c r="K6" s="45" t="s">
@@ -1576,7 +1616,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="54"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -1591,7 +1631,7 @@
       <c r="H7" s="29">
         <v>603301446</v>
       </c>
-      <c r="J7" s="54"/>
+      <c r="J7" s="61"/>
       <c r="K7" s="36" t="s">
         <v>39</v>
       </c>
@@ -1602,7 +1642,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B8" t="s">
@@ -1618,7 +1658,7 @@
         <f>(8732510/600502230)*(1066040/1226278)</f>
         <v>1.2641803364126243E-2</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="59" t="s">
         <v>36</v>
       </c>
       <c r="K8" s="45" t="s">
@@ -1633,7 +1673,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="53"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="39" t="s">
         <v>41</v>
       </c>
@@ -1649,7 +1689,7 @@
         <f>H7*H8</f>
         <v>7626818.2496250272</v>
       </c>
-      <c r="J9" s="53"/>
+      <c r="J9" s="60"/>
       <c r="K9" s="42" t="s">
         <v>41</v>
       </c>
@@ -1662,11 +1702,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="51"/>
+      <c r="J10" s="58"/>
       <c r="M10" s="46"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J11" s="51"/>
+      <c r="J11" s="58"/>
       <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1693,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477B02B9-F3EB-4652-BD38-9CEDC80D3E86}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,45 +1749,64 @@
     <col min="6" max="6" width="13.21875" customWidth="1"/>
     <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4.77734375" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" customWidth="1"/>
     <col min="10" max="10" width="6.88671875" customWidth="1"/>
     <col min="11" max="11" width="13.109375" customWidth="1"/>
     <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="3.77734375" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="F3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="61"/>
-      <c r="J3" s="60" t="s">
+      <c r="G3" s="53"/>
+      <c r="H3" s="57"/>
+      <c r="J3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="61"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="57"/>
+      <c r="O3" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="S3" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="66"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="16" t="s">
         <v>21</v>
@@ -1777,9 +1836,29 @@
       <c r="M4" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="67.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="O4" s="15"/>
+      <c r="P4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="21"/>
+      <c r="T4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="67.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="63" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1800,7 +1879,7 @@
       <c r="H5" s="23">
         <v>4.9300000000000001E-9</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="63" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="26" t="s">
@@ -1811,9 +1890,33 @@
         <f>D5/(4*H5*H6*H9)</f>
         <v>38933.688014186569</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="O5" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>1.9810499999999998E-3</v>
+      </c>
+      <c r="S5" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="27"/>
+      <c r="V5" s="69">
+        <f>(D5-2*Q5)/(4*H5*H6*H9)</f>
+        <v>38933.685379826558</v>
+      </c>
+      <c r="W5" s="70">
+        <f>(D5+2*Q5)/(4*H5*H6*H9)</f>
+        <v>38933.690648546581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="59" t="s">
         <v>28</v>
       </c>
       <c r="B6" t="s">
@@ -1832,7 +1935,7 @@
       <c r="H6" s="23">
         <v>10</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="59" t="s">
         <v>28</v>
       </c>
       <c r="K6" s="45" t="s">
@@ -1843,9 +1946,33 @@
         <f>D6*M5</f>
         <v>924558.28927288845</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="54"/>
+      <c r="O6" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="29">
+        <v>3.8511800000000001E-3</v>
+      </c>
+      <c r="S6" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="T6" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="30"/>
+      <c r="V6" s="71">
+        <f>(D6-2*Q6)*M5</f>
+        <v>924258.40799167554</v>
+      </c>
+      <c r="W6" s="31">
+        <f>(D6+2*Q6)*M5</f>
+        <v>924858.17055410135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="61"/>
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -1862,7 +1989,7 @@
       <c r="H7" s="29">
         <v>603301446</v>
       </c>
-      <c r="J7" s="54"/>
+      <c r="J7" s="61"/>
       <c r="K7" s="36" t="s">
         <v>39</v>
       </c>
@@ -1871,9 +1998,29 @@
         <f>D7*M5</f>
         <v>2565.7300401348948</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="52" t="s">
+      <c r="O7" s="61"/>
+      <c r="P7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="23">
+        <v>5.3430800000000001E-3</v>
+      </c>
+      <c r="S7" s="61"/>
+      <c r="T7" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="U7" s="37"/>
+      <c r="V7" s="72">
+        <f>(D7-2*Q7)*M5</f>
+        <v>2149.678420625215</v>
+      </c>
+      <c r="W7" s="38">
+        <f>(D7+2*Q7)*M5</f>
+        <v>2981.781659644575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B8" t="s">
@@ -1891,7 +2038,7 @@
         <f>(8732510/600502230)*(1066040/1226278)</f>
         <v>1.2641803364126243E-2</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="59" t="s">
         <v>36</v>
       </c>
       <c r="K8" s="45" t="s">
@@ -1904,9 +2051,35 @@
         <f>2*D8*M5*H6</f>
         <v>4059304.1797351204</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="53"/>
+      <c r="O8" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="29">
+        <v>2.1389400000000002E-3</v>
+      </c>
+      <c r="S8" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="U8" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="71">
+        <f>2*(D8-2*Q8)*M5*H6</f>
+        <v>4055973.1068294775</v>
+      </c>
+      <c r="W8" s="31">
+        <f>2*(D8+2*Q8)*M5*H6</f>
+        <v>4062635.2526407624</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="60"/>
       <c r="B9" s="39" t="s">
         <v>41</v>
       </c>
@@ -1924,7 +2097,7 @@
         <f>H7*H8</f>
         <v>7626818.2496250272</v>
       </c>
-      <c r="J9" s="53"/>
+      <c r="J9" s="60"/>
       <c r="K9" s="42" t="s">
         <v>41</v>
       </c>
@@ -1935,23 +2108,51 @@
         <f>2*D9*M5*H6</f>
         <v>15651.342581703</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="51"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="41">
+        <v>5.0642899999999999E-3</v>
+      </c>
+      <c r="S9" s="60"/>
+      <c r="T9" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="73">
+        <f>2*(D9-2*Q9)*M5*H6</f>
+        <v>7764.4831067684045</v>
+      </c>
+      <c r="W9" s="43">
+        <f>2*(D9+2*Q9)*M5*H6</f>
+        <v>23538.202056637598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="58"/>
       <c r="M10" s="46"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J11" s="51"/>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J11" s="58"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
       <c r="J14" s="44"/>
       <c r="M14" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="S3:W3"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="J10:J11"/>

</xml_diff>